<commit_message>
Updated DistanceInterp Data from 4/21
</commit_message>
<xml_diff>
--- a/GRIP/DistanceInterp.xlsx
+++ b/GRIP/DistanceInterp.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james_tonthat\git\FRC-2017\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james_tonthat\git\FRC-2017\GRIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="2017.04.21" sheetId="2" r:id="rId1"/>
+    <sheet name="2017.04.17" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
   <si>
     <t>RPM</t>
   </si>
@@ -103,9 +104,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -121,6 +123,2113 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2017.04.21'!$A$16:$A$106</c:f>
+              <c:strCache>
+                <c:ptCount val="91"/>
+                <c:pt idx="0">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>160</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'2017.04.21'!$A$16:$A$106</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="91"/>
+                <c:pt idx="0">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>160</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2017.04.21'!$G$16:$G$106</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="91"/>
+                <c:pt idx="0">
+                  <c:v>2510.1160220994475</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2519.232044198895</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2528.3480662983425</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2537.46408839779</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2546.5801104972375</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2555.6961325966849</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2564.8121546961324</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2573.9281767955799</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2583.0441988950274</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2592.1602209944749</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2601.8988902589394</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2615.4623921085081</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2629.0258939580763</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2642.5893958076449</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2656.1528976572135</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2669.7163995067817</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2683.2799013563504</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2696.8434032059185</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2710.0331125827815</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2711.1368653421632</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2712.2406181015454</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2713.344370860927</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2714.4481236203092</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2721.3888888888887</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2734.1666666666665</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2746.9444444444443</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2759.7222222222222</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2772.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2785.2777777777778</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2798.0555555555557</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2810.8333333333335</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2823.6111111111113</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2835.5128205128203</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2846.5384615384614</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2857.5641025641025</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2868.5897435897436</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2879.6153846153848</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2890.6410256410259</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2901.6666666666665</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2912.6923076923076</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2923.7179487179487</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2934.7435897435898</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2945.7692307692309</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2956.7948717948716</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2967.8205128205127</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2978.8461538461538</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2989.8717948717949</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>3000.897435897436</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3011.9230769230771</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>3022.9487179487178</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>3033.9743589743589</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3045</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3055</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3065</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3075</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>3085</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3095</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3105</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3115</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3125</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>3135</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>3149.5604395604396</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>3164.1208791208792</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>3178.6813186813188</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>3193.2417582417584</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>3207.802197802198</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>3222.3626373626375</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>3236.9230769230771</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>3251.4835164835167</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>3266.0439560439563</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>3280.6043956043959</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>3295.1648351648355</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>3309.7252747252746</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>3324.2857142857142</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>3338.8461538461538</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>3353.4065934065934</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>3367.967032967033</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>3382.5274725274726</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>3397.0879120879122</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>3411.6437500000002</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>3426.1984375000002</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>3440.7531250000002</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>3455.3078125000002</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>3469.8625000000002</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>3484.4171875000002</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>3498.9718750000002</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>3513.5265625000002</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>3528.0812500000002</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>3542.6359375000002</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>3557.1906250000002</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>3571.7453125000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000005B-234C-4472-979D-211151C982F9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2017.04.21'!$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>70</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'2017.04.21'!$A$16:$A$106</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="91"/>
+                <c:pt idx="0">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>160</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2017.04.17'!$G$15:$G$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>2510.1160220994475</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2519.232044198895</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2528.3480662983425</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2537.46408839779</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2546.5801104972375</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2555.6961325966849</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2564.8121546961324</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2573.9281767955799</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2583.0441988950274</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2592.1602209944749</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2601.2737341772154</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2610.371835443038</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2619.4699367088606</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2628.5680379746836</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2637.6661392405063</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2646.7642405063293</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2655.8623417721519</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2664.9604430379745</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2674.0585443037976</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2683.1566455696202</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2692.2547468354433</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2701.3528481012659</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2710.4509493670885</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2721.3888888888887</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2734.1666666666665</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2746.9444444444443</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2759.7222222222222</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2772.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2785.2777777777778</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2798.0555555555557</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2810.8333333333335</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2823.6111111111113</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2836.3884210526317</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2849.165263157895</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2861.9421052631578</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2874.7189473684211</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2887.4957894736845</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2900.2726315789473</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2913.0494736842106</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2925.8263157894739</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2938.6031578947368</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000005C-234C-4472-979D-211151C982F9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="420615680"/>
+        <c:axId val="420609120"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="420615680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="420609120"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="420609120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="420615680"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>503464</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>70757</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>-1</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>136071</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C81A22DA-AAB1-4621-ADF8-0FD6D289D758}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -420,9 +2529,2783 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I107"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K99" sqref="K99"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>69</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2501</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>79.86</v>
+      </c>
+      <c r="B3">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>87.97</v>
+      </c>
+      <c r="B4">
+        <v>2710</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>92.5</v>
+      </c>
+      <c r="B5">
+        <v>2715</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>101.5</v>
+      </c>
+      <c r="B6">
+        <v>2830</v>
+      </c>
+      <c r="I6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>121</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3045</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>130</v>
+      </c>
+      <c r="B8">
+        <v>3135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>148.19999999999999</v>
+      </c>
+      <c r="B9">
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>161</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3586.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>70</v>
+      </c>
+      <c r="B16">
+        <f>INDEX($A$2:$A$10,MATCH(A16,$A$2:$A$10,1))</f>
+        <v>69</v>
+      </c>
+      <c r="C16">
+        <f>INDEX($B$2:$B$10,MATCH(A16,$A$2:$A$10,1))</f>
+        <v>2501</v>
+      </c>
+      <c r="D16">
+        <f>INDEX($A$2:$A$10,MATCH(A16,$A$2:$A$10,1)+1)</f>
+        <v>79.86</v>
+      </c>
+      <c r="E16">
+        <f>INDEX($B$2:$B$10,MATCH(A16,$A$2:$A$10,1)+1)</f>
+        <v>2600</v>
+      </c>
+      <c r="G16">
+        <f>C16+(A16-B16)*(E16-C16)/(D16-B16)</f>
+        <v>2510.1160220994475</v>
+      </c>
+      <c r="I16" t="str">
+        <f>ROUNDDOWN(G16,0)&amp;","</f>
+        <v>2510,</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>71</v>
+      </c>
+      <c r="B17">
+        <f t="shared" ref="B17:B80" si="0">INDEX($A$2:$A$10,MATCH(A17,$A$2:$A$10,1))</f>
+        <v>69</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ref="C17:C80" si="1">INDEX($B$2:$B$10,MATCH(A17,$A$2:$A$10,1))</f>
+        <v>2501</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ref="D17:D80" si="2">INDEX($A$2:$A$10,MATCH(A17,$A$2:$A$10,1)+1)</f>
+        <v>79.86</v>
+      </c>
+      <c r="E17">
+        <f t="shared" ref="E17:E80" si="3">INDEX($B$2:$B$10,MATCH(A17,$A$2:$A$10,1)+1)</f>
+        <v>2600</v>
+      </c>
+      <c r="G17">
+        <f t="shared" ref="G17:G80" si="4">C17+(A17-B17)*(E17-C17)/(D17-B17)</f>
+        <v>2519.232044198895</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" ref="I17:I80" si="5">ROUNDDOWN(G17,0)&amp;","</f>
+        <v>2519,</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>72</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>2501</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="2"/>
+        <v>79.86</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="3"/>
+        <v>2600</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="4"/>
+        <v>2528.3480662983425</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="5"/>
+        <v>2528,</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>73</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>2501</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="2"/>
+        <v>79.86</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="3"/>
+        <v>2600</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="4"/>
+        <v>2537.46408839779</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="5"/>
+        <v>2537,</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>74</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>2501</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="2"/>
+        <v>79.86</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="3"/>
+        <v>2600</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="4"/>
+        <v>2546.5801104972375</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="5"/>
+        <v>2546,</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>75</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>2501</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="2"/>
+        <v>79.86</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="3"/>
+        <v>2600</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="4"/>
+        <v>2555.6961325966849</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="5"/>
+        <v>2555,</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>76</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>2501</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="2"/>
+        <v>79.86</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="3"/>
+        <v>2600</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="4"/>
+        <v>2564.8121546961324</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="5"/>
+        <v>2564,</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>77</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>2501</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="2"/>
+        <v>79.86</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="3"/>
+        <v>2600</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="4"/>
+        <v>2573.9281767955799</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="5"/>
+        <v>2573,</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>78</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
+        <v>2501</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="2"/>
+        <v>79.86</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="3"/>
+        <v>2600</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="4"/>
+        <v>2583.0441988950274</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="5"/>
+        <v>2583,</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>79</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>2501</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="2"/>
+        <v>79.86</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="3"/>
+        <v>2600</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="4"/>
+        <v>2592.1602209944749</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="5"/>
+        <v>2592,</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>80</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>79.86</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>2600</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="2"/>
+        <v>87.97</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="3"/>
+        <v>2710</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="4"/>
+        <v>2601.8988902589394</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="5"/>
+        <v>2601,</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>81</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>79.86</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="1"/>
+        <v>2600</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="2"/>
+        <v>87.97</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="3"/>
+        <v>2710</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="4"/>
+        <v>2615.4623921085081</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="5"/>
+        <v>2615,</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>82</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>79.86</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="1"/>
+        <v>2600</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="2"/>
+        <v>87.97</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="3"/>
+        <v>2710</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="4"/>
+        <v>2629.0258939580763</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="5"/>
+        <v>2629,</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>83</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>79.86</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="1"/>
+        <v>2600</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="2"/>
+        <v>87.97</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="3"/>
+        <v>2710</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="4"/>
+        <v>2642.5893958076449</v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="5"/>
+        <v>2642,</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>84</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>79.86</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="1"/>
+        <v>2600</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="2"/>
+        <v>87.97</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="3"/>
+        <v>2710</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="4"/>
+        <v>2656.1528976572135</v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="5"/>
+        <v>2656,</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>85</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>79.86</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="1"/>
+        <v>2600</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="2"/>
+        <v>87.97</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="3"/>
+        <v>2710</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="4"/>
+        <v>2669.7163995067817</v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="5"/>
+        <v>2669,</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>86</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>79.86</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="1"/>
+        <v>2600</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="2"/>
+        <v>87.97</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="3"/>
+        <v>2710</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="4"/>
+        <v>2683.2799013563504</v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" si="5"/>
+        <v>2683,</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>87</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>79.86</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="1"/>
+        <v>2600</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="2"/>
+        <v>87.97</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="3"/>
+        <v>2710</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="4"/>
+        <v>2696.8434032059185</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="5"/>
+        <v>2696,</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>88</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>87.97</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="1"/>
+        <v>2710</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="2"/>
+        <v>92.5</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="3"/>
+        <v>2715</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="4"/>
+        <v>2710.0331125827815</v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="5"/>
+        <v>2710,</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>89</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>87.97</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="1"/>
+        <v>2710</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="2"/>
+        <v>92.5</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="3"/>
+        <v>2715</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="4"/>
+        <v>2711.1368653421632</v>
+      </c>
+      <c r="I35" t="str">
+        <f t="shared" si="5"/>
+        <v>2711,</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>90</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>87.97</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="1"/>
+        <v>2710</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="2"/>
+        <v>92.5</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="3"/>
+        <v>2715</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="4"/>
+        <v>2712.2406181015454</v>
+      </c>
+      <c r="I36" t="str">
+        <f t="shared" si="5"/>
+        <v>2712,</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>91</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>87.97</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="1"/>
+        <v>2710</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="2"/>
+        <v>92.5</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="3"/>
+        <v>2715</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="4"/>
+        <v>2713.344370860927</v>
+      </c>
+      <c r="I37" t="str">
+        <f t="shared" si="5"/>
+        <v>2713,</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>92</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>87.97</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="1"/>
+        <v>2710</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="2"/>
+        <v>92.5</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="3"/>
+        <v>2715</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="4"/>
+        <v>2714.4481236203092</v>
+      </c>
+      <c r="I38" t="str">
+        <f t="shared" si="5"/>
+        <v>2714,</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>93</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>92.5</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="1"/>
+        <v>2715</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="2"/>
+        <v>101.5</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="3"/>
+        <v>2830</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="4"/>
+        <v>2721.3888888888887</v>
+      </c>
+      <c r="I39" t="str">
+        <f t="shared" si="5"/>
+        <v>2721,</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>94</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>92.5</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="1"/>
+        <v>2715</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="2"/>
+        <v>101.5</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="3"/>
+        <v>2830</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="4"/>
+        <v>2734.1666666666665</v>
+      </c>
+      <c r="I40" t="str">
+        <f t="shared" si="5"/>
+        <v>2734,</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>95</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>92.5</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="1"/>
+        <v>2715</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="2"/>
+        <v>101.5</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="3"/>
+        <v>2830</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="4"/>
+        <v>2746.9444444444443</v>
+      </c>
+      <c r="I41" t="str">
+        <f t="shared" si="5"/>
+        <v>2746,</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>96</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>92.5</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="1"/>
+        <v>2715</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="2"/>
+        <v>101.5</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="3"/>
+        <v>2830</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="4"/>
+        <v>2759.7222222222222</v>
+      </c>
+      <c r="I42" t="str">
+        <f t="shared" si="5"/>
+        <v>2759,</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>97</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="0"/>
+        <v>92.5</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="1"/>
+        <v>2715</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="2"/>
+        <v>101.5</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="3"/>
+        <v>2830</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="4"/>
+        <v>2772.5</v>
+      </c>
+      <c r="I43" t="str">
+        <f t="shared" si="5"/>
+        <v>2772,</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>98</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="0"/>
+        <v>92.5</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="1"/>
+        <v>2715</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="2"/>
+        <v>101.5</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="3"/>
+        <v>2830</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="4"/>
+        <v>2785.2777777777778</v>
+      </c>
+      <c r="I44" t="str">
+        <f t="shared" si="5"/>
+        <v>2785,</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>99</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="0"/>
+        <v>92.5</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="1"/>
+        <v>2715</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="2"/>
+        <v>101.5</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="3"/>
+        <v>2830</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="4"/>
+        <v>2798.0555555555557</v>
+      </c>
+      <c r="I45" t="str">
+        <f t="shared" si="5"/>
+        <v>2798,</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>100</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="0"/>
+        <v>92.5</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="1"/>
+        <v>2715</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="2"/>
+        <v>101.5</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="3"/>
+        <v>2830</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="4"/>
+        <v>2810.8333333333335</v>
+      </c>
+      <c r="I46" t="str">
+        <f t="shared" si="5"/>
+        <v>2810,</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>101</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="0"/>
+        <v>92.5</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="1"/>
+        <v>2715</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="2"/>
+        <v>101.5</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="3"/>
+        <v>2830</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="4"/>
+        <v>2823.6111111111113</v>
+      </c>
+      <c r="I47" t="str">
+        <f t="shared" si="5"/>
+        <v>2823,</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>102</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="0"/>
+        <v>101.5</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="1"/>
+        <v>2830</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="2"/>
+        <v>121</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="3"/>
+        <v>3045</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="4"/>
+        <v>2835.5128205128203</v>
+      </c>
+      <c r="I48" t="str">
+        <f t="shared" si="5"/>
+        <v>2835,</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>103</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="0"/>
+        <v>101.5</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="1"/>
+        <v>2830</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="2"/>
+        <v>121</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="3"/>
+        <v>3045</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="4"/>
+        <v>2846.5384615384614</v>
+      </c>
+      <c r="I49" t="str">
+        <f t="shared" si="5"/>
+        <v>2846,</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>104</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="0"/>
+        <v>101.5</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="1"/>
+        <v>2830</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="2"/>
+        <v>121</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="3"/>
+        <v>3045</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="4"/>
+        <v>2857.5641025641025</v>
+      </c>
+      <c r="I50" t="str">
+        <f t="shared" si="5"/>
+        <v>2857,</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>105</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="0"/>
+        <v>101.5</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="1"/>
+        <v>2830</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="2"/>
+        <v>121</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="3"/>
+        <v>3045</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="4"/>
+        <v>2868.5897435897436</v>
+      </c>
+      <c r="I51" t="str">
+        <f t="shared" si="5"/>
+        <v>2868,</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>106</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="0"/>
+        <v>101.5</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="1"/>
+        <v>2830</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="2"/>
+        <v>121</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="3"/>
+        <v>3045</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="4"/>
+        <v>2879.6153846153848</v>
+      </c>
+      <c r="I52" t="str">
+        <f t="shared" si="5"/>
+        <v>2879,</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>107</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="0"/>
+        <v>101.5</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="1"/>
+        <v>2830</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="2"/>
+        <v>121</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="3"/>
+        <v>3045</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="4"/>
+        <v>2890.6410256410259</v>
+      </c>
+      <c r="I53" t="str">
+        <f t="shared" si="5"/>
+        <v>2890,</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>108</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="0"/>
+        <v>101.5</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="1"/>
+        <v>2830</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="2"/>
+        <v>121</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="3"/>
+        <v>3045</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="4"/>
+        <v>2901.6666666666665</v>
+      </c>
+      <c r="I54" t="str">
+        <f t="shared" si="5"/>
+        <v>2901,</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>109</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="0"/>
+        <v>101.5</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="1"/>
+        <v>2830</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="2"/>
+        <v>121</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="3"/>
+        <v>3045</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="4"/>
+        <v>2912.6923076923076</v>
+      </c>
+      <c r="I55" t="str">
+        <f t="shared" si="5"/>
+        <v>2912,</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>110</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="0"/>
+        <v>101.5</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="1"/>
+        <v>2830</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="2"/>
+        <v>121</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="3"/>
+        <v>3045</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="4"/>
+        <v>2923.7179487179487</v>
+      </c>
+      <c r="I56" t="str">
+        <f t="shared" si="5"/>
+        <v>2923,</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>111</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="0"/>
+        <v>101.5</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="1"/>
+        <v>2830</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="2"/>
+        <v>121</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="3"/>
+        <v>3045</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="4"/>
+        <v>2934.7435897435898</v>
+      </c>
+      <c r="I57" t="str">
+        <f t="shared" si="5"/>
+        <v>2934,</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>112</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="0"/>
+        <v>101.5</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="1"/>
+        <v>2830</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="2"/>
+        <v>121</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="3"/>
+        <v>3045</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="4"/>
+        <v>2945.7692307692309</v>
+      </c>
+      <c r="I58" t="str">
+        <f t="shared" si="5"/>
+        <v>2945,</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>113</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="0"/>
+        <v>101.5</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="1"/>
+        <v>2830</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="2"/>
+        <v>121</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="3"/>
+        <v>3045</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="4"/>
+        <v>2956.7948717948716</v>
+      </c>
+      <c r="I59" t="str">
+        <f t="shared" si="5"/>
+        <v>2956,</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>114</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="0"/>
+        <v>101.5</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="1"/>
+        <v>2830</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="2"/>
+        <v>121</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="3"/>
+        <v>3045</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="4"/>
+        <v>2967.8205128205127</v>
+      </c>
+      <c r="I60" t="str">
+        <f t="shared" si="5"/>
+        <v>2967,</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>115</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="0"/>
+        <v>101.5</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="1"/>
+        <v>2830</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="2"/>
+        <v>121</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="3"/>
+        <v>3045</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="4"/>
+        <v>2978.8461538461538</v>
+      </c>
+      <c r="I61" t="str">
+        <f t="shared" si="5"/>
+        <v>2978,</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>116</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="0"/>
+        <v>101.5</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="1"/>
+        <v>2830</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="2"/>
+        <v>121</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="3"/>
+        <v>3045</v>
+      </c>
+      <c r="G62">
+        <f t="shared" si="4"/>
+        <v>2989.8717948717949</v>
+      </c>
+      <c r="I62" t="str">
+        <f t="shared" si="5"/>
+        <v>2989,</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>117</v>
+      </c>
+      <c r="B63">
+        <f t="shared" si="0"/>
+        <v>101.5</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="1"/>
+        <v>2830</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="2"/>
+        <v>121</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="3"/>
+        <v>3045</v>
+      </c>
+      <c r="G63">
+        <f t="shared" si="4"/>
+        <v>3000.897435897436</v>
+      </c>
+      <c r="I63" t="str">
+        <f t="shared" si="5"/>
+        <v>3000,</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>118</v>
+      </c>
+      <c r="B64">
+        <f t="shared" si="0"/>
+        <v>101.5</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="1"/>
+        <v>2830</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="2"/>
+        <v>121</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="3"/>
+        <v>3045</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="4"/>
+        <v>3011.9230769230771</v>
+      </c>
+      <c r="I64" t="str">
+        <f t="shared" si="5"/>
+        <v>3011,</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>119</v>
+      </c>
+      <c r="B65">
+        <f t="shared" si="0"/>
+        <v>101.5</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="1"/>
+        <v>2830</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="2"/>
+        <v>121</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="3"/>
+        <v>3045</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="4"/>
+        <v>3022.9487179487178</v>
+      </c>
+      <c r="I65" t="str">
+        <f t="shared" si="5"/>
+        <v>3022,</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>120</v>
+      </c>
+      <c r="B66">
+        <f t="shared" si="0"/>
+        <v>101.5</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="1"/>
+        <v>2830</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="2"/>
+        <v>121</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="3"/>
+        <v>3045</v>
+      </c>
+      <c r="G66">
+        <f t="shared" si="4"/>
+        <v>3033.9743589743589</v>
+      </c>
+      <c r="I66" t="str">
+        <f t="shared" si="5"/>
+        <v>3033,</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>121</v>
+      </c>
+      <c r="B67">
+        <f t="shared" si="0"/>
+        <v>121</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="1"/>
+        <v>3045</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="2"/>
+        <v>130</v>
+      </c>
+      <c r="E67">
+        <f t="shared" si="3"/>
+        <v>3135</v>
+      </c>
+      <c r="G67">
+        <f t="shared" si="4"/>
+        <v>3045</v>
+      </c>
+      <c r="I67" t="str">
+        <f t="shared" si="5"/>
+        <v>3045,</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>122</v>
+      </c>
+      <c r="B68">
+        <f t="shared" si="0"/>
+        <v>121</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="1"/>
+        <v>3045</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="2"/>
+        <v>130</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="3"/>
+        <v>3135</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="4"/>
+        <v>3055</v>
+      </c>
+      <c r="I68" t="str">
+        <f t="shared" si="5"/>
+        <v>3055,</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>123</v>
+      </c>
+      <c r="B69">
+        <f t="shared" si="0"/>
+        <v>121</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="1"/>
+        <v>3045</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="2"/>
+        <v>130</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="3"/>
+        <v>3135</v>
+      </c>
+      <c r="G69">
+        <f t="shared" si="4"/>
+        <v>3065</v>
+      </c>
+      <c r="I69" t="str">
+        <f t="shared" si="5"/>
+        <v>3065,</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>124</v>
+      </c>
+      <c r="B70">
+        <f t="shared" si="0"/>
+        <v>121</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="1"/>
+        <v>3045</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="2"/>
+        <v>130</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="3"/>
+        <v>3135</v>
+      </c>
+      <c r="G70">
+        <f t="shared" si="4"/>
+        <v>3075</v>
+      </c>
+      <c r="I70" t="str">
+        <f t="shared" si="5"/>
+        <v>3075,</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>125</v>
+      </c>
+      <c r="B71">
+        <f t="shared" si="0"/>
+        <v>121</v>
+      </c>
+      <c r="C71">
+        <f t="shared" si="1"/>
+        <v>3045</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="2"/>
+        <v>130</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="3"/>
+        <v>3135</v>
+      </c>
+      <c r="G71">
+        <f t="shared" si="4"/>
+        <v>3085</v>
+      </c>
+      <c r="I71" t="str">
+        <f t="shared" si="5"/>
+        <v>3085,</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>126</v>
+      </c>
+      <c r="B72">
+        <f t="shared" si="0"/>
+        <v>121</v>
+      </c>
+      <c r="C72">
+        <f t="shared" si="1"/>
+        <v>3045</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="2"/>
+        <v>130</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="3"/>
+        <v>3135</v>
+      </c>
+      <c r="G72">
+        <f t="shared" si="4"/>
+        <v>3095</v>
+      </c>
+      <c r="I72" t="str">
+        <f t="shared" si="5"/>
+        <v>3095,</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>127</v>
+      </c>
+      <c r="B73">
+        <f t="shared" si="0"/>
+        <v>121</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="1"/>
+        <v>3045</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="2"/>
+        <v>130</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="3"/>
+        <v>3135</v>
+      </c>
+      <c r="G73">
+        <f t="shared" si="4"/>
+        <v>3105</v>
+      </c>
+      <c r="I73" t="str">
+        <f t="shared" si="5"/>
+        <v>3105,</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>128</v>
+      </c>
+      <c r="B74">
+        <f t="shared" si="0"/>
+        <v>121</v>
+      </c>
+      <c r="C74">
+        <f t="shared" si="1"/>
+        <v>3045</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="2"/>
+        <v>130</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="3"/>
+        <v>3135</v>
+      </c>
+      <c r="G74">
+        <f t="shared" si="4"/>
+        <v>3115</v>
+      </c>
+      <c r="I74" t="str">
+        <f t="shared" si="5"/>
+        <v>3115,</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>129</v>
+      </c>
+      <c r="B75">
+        <f t="shared" si="0"/>
+        <v>121</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="1"/>
+        <v>3045</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="2"/>
+        <v>130</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="3"/>
+        <v>3135</v>
+      </c>
+      <c r="G75">
+        <f t="shared" si="4"/>
+        <v>3125</v>
+      </c>
+      <c r="I75" t="str">
+        <f t="shared" si="5"/>
+        <v>3125,</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>130</v>
+      </c>
+      <c r="B76">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="1"/>
+        <v>3135</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="2"/>
+        <v>148.19999999999999</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="3"/>
+        <v>3400</v>
+      </c>
+      <c r="G76">
+        <f t="shared" si="4"/>
+        <v>3135</v>
+      </c>
+      <c r="I76" t="str">
+        <f t="shared" si="5"/>
+        <v>3135,</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>131</v>
+      </c>
+      <c r="B77">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="1"/>
+        <v>3135</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="2"/>
+        <v>148.19999999999999</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="3"/>
+        <v>3400</v>
+      </c>
+      <c r="G77">
+        <f t="shared" si="4"/>
+        <v>3149.5604395604396</v>
+      </c>
+      <c r="I77" t="str">
+        <f t="shared" si="5"/>
+        <v>3149,</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>132</v>
+      </c>
+      <c r="B78">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="1"/>
+        <v>3135</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="2"/>
+        <v>148.19999999999999</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="3"/>
+        <v>3400</v>
+      </c>
+      <c r="G78">
+        <f t="shared" si="4"/>
+        <v>3164.1208791208792</v>
+      </c>
+      <c r="I78" t="str">
+        <f t="shared" si="5"/>
+        <v>3164,</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>133</v>
+      </c>
+      <c r="B79">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="1"/>
+        <v>3135</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="2"/>
+        <v>148.19999999999999</v>
+      </c>
+      <c r="E79">
+        <f t="shared" si="3"/>
+        <v>3400</v>
+      </c>
+      <c r="G79">
+        <f t="shared" si="4"/>
+        <v>3178.6813186813188</v>
+      </c>
+      <c r="I79" t="str">
+        <f t="shared" si="5"/>
+        <v>3178,</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>134</v>
+      </c>
+      <c r="B80">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="C80">
+        <f t="shared" si="1"/>
+        <v>3135</v>
+      </c>
+      <c r="D80">
+        <f t="shared" si="2"/>
+        <v>148.19999999999999</v>
+      </c>
+      <c r="E80">
+        <f t="shared" si="3"/>
+        <v>3400</v>
+      </c>
+      <c r="G80">
+        <f t="shared" si="4"/>
+        <v>3193.2417582417584</v>
+      </c>
+      <c r="I80" t="str">
+        <f t="shared" si="5"/>
+        <v>3193,</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>135</v>
+      </c>
+      <c r="B81">
+        <f t="shared" ref="B81:B106" si="6">INDEX($A$2:$A$10,MATCH(A81,$A$2:$A$10,1))</f>
+        <v>130</v>
+      </c>
+      <c r="C81">
+        <f t="shared" ref="C81:C106" si="7">INDEX($B$2:$B$10,MATCH(A81,$A$2:$A$10,1))</f>
+        <v>3135</v>
+      </c>
+      <c r="D81">
+        <f t="shared" ref="D81:D106" si="8">INDEX($A$2:$A$10,MATCH(A81,$A$2:$A$10,1)+1)</f>
+        <v>148.19999999999999</v>
+      </c>
+      <c r="E81">
+        <f t="shared" ref="E81:E106" si="9">INDEX($B$2:$B$10,MATCH(A81,$A$2:$A$10,1)+1)</f>
+        <v>3400</v>
+      </c>
+      <c r="G81">
+        <f t="shared" ref="G81:G106" si="10">C81+(A81-B81)*(E81-C81)/(D81-B81)</f>
+        <v>3207.802197802198</v>
+      </c>
+      <c r="I81" t="str">
+        <f t="shared" ref="I81:I106" si="11">ROUNDDOWN(G81,0)&amp;","</f>
+        <v>3207,</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>136</v>
+      </c>
+      <c r="B82">
+        <f t="shared" si="6"/>
+        <v>130</v>
+      </c>
+      <c r="C82">
+        <f t="shared" si="7"/>
+        <v>3135</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="8"/>
+        <v>148.19999999999999</v>
+      </c>
+      <c r="E82">
+        <f t="shared" si="9"/>
+        <v>3400</v>
+      </c>
+      <c r="G82">
+        <f t="shared" si="10"/>
+        <v>3222.3626373626375</v>
+      </c>
+      <c r="I82" t="str">
+        <f t="shared" si="11"/>
+        <v>3222,</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>137</v>
+      </c>
+      <c r="B83">
+        <f t="shared" si="6"/>
+        <v>130</v>
+      </c>
+      <c r="C83">
+        <f t="shared" si="7"/>
+        <v>3135</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="8"/>
+        <v>148.19999999999999</v>
+      </c>
+      <c r="E83">
+        <f t="shared" si="9"/>
+        <v>3400</v>
+      </c>
+      <c r="G83">
+        <f t="shared" si="10"/>
+        <v>3236.9230769230771</v>
+      </c>
+      <c r="I83" t="str">
+        <f t="shared" si="11"/>
+        <v>3236,</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>138</v>
+      </c>
+      <c r="B84">
+        <f t="shared" si="6"/>
+        <v>130</v>
+      </c>
+      <c r="C84">
+        <f t="shared" si="7"/>
+        <v>3135</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="8"/>
+        <v>148.19999999999999</v>
+      </c>
+      <c r="E84">
+        <f t="shared" si="9"/>
+        <v>3400</v>
+      </c>
+      <c r="G84">
+        <f t="shared" si="10"/>
+        <v>3251.4835164835167</v>
+      </c>
+      <c r="I84" t="str">
+        <f t="shared" si="11"/>
+        <v>3251,</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>139</v>
+      </c>
+      <c r="B85">
+        <f t="shared" si="6"/>
+        <v>130</v>
+      </c>
+      <c r="C85">
+        <f t="shared" si="7"/>
+        <v>3135</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="8"/>
+        <v>148.19999999999999</v>
+      </c>
+      <c r="E85">
+        <f t="shared" si="9"/>
+        <v>3400</v>
+      </c>
+      <c r="G85">
+        <f t="shared" si="10"/>
+        <v>3266.0439560439563</v>
+      </c>
+      <c r="I85" t="str">
+        <f t="shared" si="11"/>
+        <v>3266,</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>140</v>
+      </c>
+      <c r="B86">
+        <f t="shared" si="6"/>
+        <v>130</v>
+      </c>
+      <c r="C86">
+        <f t="shared" si="7"/>
+        <v>3135</v>
+      </c>
+      <c r="D86">
+        <f t="shared" si="8"/>
+        <v>148.19999999999999</v>
+      </c>
+      <c r="E86">
+        <f t="shared" si="9"/>
+        <v>3400</v>
+      </c>
+      <c r="G86">
+        <f t="shared" si="10"/>
+        <v>3280.6043956043959</v>
+      </c>
+      <c r="I86" t="str">
+        <f t="shared" si="11"/>
+        <v>3280,</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>141</v>
+      </c>
+      <c r="B87">
+        <f t="shared" si="6"/>
+        <v>130</v>
+      </c>
+      <c r="C87">
+        <f t="shared" si="7"/>
+        <v>3135</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="8"/>
+        <v>148.19999999999999</v>
+      </c>
+      <c r="E87">
+        <f t="shared" si="9"/>
+        <v>3400</v>
+      </c>
+      <c r="G87">
+        <f t="shared" si="10"/>
+        <v>3295.1648351648355</v>
+      </c>
+      <c r="I87" t="str">
+        <f t="shared" si="11"/>
+        <v>3295,</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>142</v>
+      </c>
+      <c r="B88">
+        <f t="shared" si="6"/>
+        <v>130</v>
+      </c>
+      <c r="C88">
+        <f t="shared" si="7"/>
+        <v>3135</v>
+      </c>
+      <c r="D88">
+        <f t="shared" si="8"/>
+        <v>148.19999999999999</v>
+      </c>
+      <c r="E88">
+        <f t="shared" si="9"/>
+        <v>3400</v>
+      </c>
+      <c r="G88">
+        <f t="shared" si="10"/>
+        <v>3309.7252747252746</v>
+      </c>
+      <c r="I88" t="str">
+        <f t="shared" si="11"/>
+        <v>3309,</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>143</v>
+      </c>
+      <c r="B89">
+        <f t="shared" si="6"/>
+        <v>130</v>
+      </c>
+      <c r="C89">
+        <f t="shared" si="7"/>
+        <v>3135</v>
+      </c>
+      <c r="D89">
+        <f t="shared" si="8"/>
+        <v>148.19999999999999</v>
+      </c>
+      <c r="E89">
+        <f t="shared" si="9"/>
+        <v>3400</v>
+      </c>
+      <c r="G89">
+        <f t="shared" si="10"/>
+        <v>3324.2857142857142</v>
+      </c>
+      <c r="I89" t="str">
+        <f t="shared" si="11"/>
+        <v>3324,</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>144</v>
+      </c>
+      <c r="B90">
+        <f t="shared" si="6"/>
+        <v>130</v>
+      </c>
+      <c r="C90">
+        <f t="shared" si="7"/>
+        <v>3135</v>
+      </c>
+      <c r="D90">
+        <f t="shared" si="8"/>
+        <v>148.19999999999999</v>
+      </c>
+      <c r="E90">
+        <f t="shared" si="9"/>
+        <v>3400</v>
+      </c>
+      <c r="G90">
+        <f t="shared" si="10"/>
+        <v>3338.8461538461538</v>
+      </c>
+      <c r="I90" t="str">
+        <f t="shared" si="11"/>
+        <v>3338,</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>145</v>
+      </c>
+      <c r="B91">
+        <f t="shared" si="6"/>
+        <v>130</v>
+      </c>
+      <c r="C91">
+        <f t="shared" si="7"/>
+        <v>3135</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="8"/>
+        <v>148.19999999999999</v>
+      </c>
+      <c r="E91">
+        <f t="shared" si="9"/>
+        <v>3400</v>
+      </c>
+      <c r="G91">
+        <f t="shared" si="10"/>
+        <v>3353.4065934065934</v>
+      </c>
+      <c r="I91" t="str">
+        <f t="shared" si="11"/>
+        <v>3353,</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>146</v>
+      </c>
+      <c r="B92">
+        <f t="shared" si="6"/>
+        <v>130</v>
+      </c>
+      <c r="C92">
+        <f t="shared" si="7"/>
+        <v>3135</v>
+      </c>
+      <c r="D92">
+        <f t="shared" si="8"/>
+        <v>148.19999999999999</v>
+      </c>
+      <c r="E92">
+        <f t="shared" si="9"/>
+        <v>3400</v>
+      </c>
+      <c r="G92">
+        <f t="shared" si="10"/>
+        <v>3367.967032967033</v>
+      </c>
+      <c r="I92" t="str">
+        <f t="shared" si="11"/>
+        <v>3367,</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>147</v>
+      </c>
+      <c r="B93">
+        <f t="shared" si="6"/>
+        <v>130</v>
+      </c>
+      <c r="C93">
+        <f t="shared" si="7"/>
+        <v>3135</v>
+      </c>
+      <c r="D93">
+        <f t="shared" si="8"/>
+        <v>148.19999999999999</v>
+      </c>
+      <c r="E93">
+        <f t="shared" si="9"/>
+        <v>3400</v>
+      </c>
+      <c r="G93">
+        <f t="shared" si="10"/>
+        <v>3382.5274725274726</v>
+      </c>
+      <c r="I93" t="str">
+        <f t="shared" si="11"/>
+        <v>3382,</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>148</v>
+      </c>
+      <c r="B94">
+        <f t="shared" si="6"/>
+        <v>130</v>
+      </c>
+      <c r="C94">
+        <f t="shared" si="7"/>
+        <v>3135</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="8"/>
+        <v>148.19999999999999</v>
+      </c>
+      <c r="E94">
+        <f t="shared" si="9"/>
+        <v>3400</v>
+      </c>
+      <c r="G94">
+        <f t="shared" si="10"/>
+        <v>3397.0879120879122</v>
+      </c>
+      <c r="I94" t="str">
+        <f t="shared" si="11"/>
+        <v>3397,</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>149</v>
+      </c>
+      <c r="B95">
+        <f t="shared" si="6"/>
+        <v>148.19999999999999</v>
+      </c>
+      <c r="C95">
+        <f t="shared" si="7"/>
+        <v>3400</v>
+      </c>
+      <c r="D95">
+        <f t="shared" si="8"/>
+        <v>161</v>
+      </c>
+      <c r="E95">
+        <f t="shared" si="9"/>
+        <v>3586.3</v>
+      </c>
+      <c r="G95">
+        <f t="shared" si="10"/>
+        <v>3411.6437500000002</v>
+      </c>
+      <c r="I95" t="str">
+        <f t="shared" si="11"/>
+        <v>3411,</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>150</v>
+      </c>
+      <c r="B96">
+        <f t="shared" si="6"/>
+        <v>148.19999999999999</v>
+      </c>
+      <c r="C96">
+        <f t="shared" si="7"/>
+        <v>3400</v>
+      </c>
+      <c r="D96">
+        <f t="shared" si="8"/>
+        <v>161</v>
+      </c>
+      <c r="E96">
+        <f t="shared" si="9"/>
+        <v>3586.3</v>
+      </c>
+      <c r="G96">
+        <f t="shared" si="10"/>
+        <v>3426.1984375000002</v>
+      </c>
+      <c r="I96" t="str">
+        <f t="shared" si="11"/>
+        <v>3426,</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>151</v>
+      </c>
+      <c r="B97">
+        <f t="shared" si="6"/>
+        <v>148.19999999999999</v>
+      </c>
+      <c r="C97">
+        <f t="shared" si="7"/>
+        <v>3400</v>
+      </c>
+      <c r="D97">
+        <f t="shared" si="8"/>
+        <v>161</v>
+      </c>
+      <c r="E97">
+        <f t="shared" si="9"/>
+        <v>3586.3</v>
+      </c>
+      <c r="G97">
+        <f t="shared" si="10"/>
+        <v>3440.7531250000002</v>
+      </c>
+      <c r="I97" t="str">
+        <f t="shared" si="11"/>
+        <v>3440,</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>152</v>
+      </c>
+      <c r="B98">
+        <f t="shared" si="6"/>
+        <v>148.19999999999999</v>
+      </c>
+      <c r="C98">
+        <f t="shared" si="7"/>
+        <v>3400</v>
+      </c>
+      <c r="D98">
+        <f t="shared" si="8"/>
+        <v>161</v>
+      </c>
+      <c r="E98">
+        <f t="shared" si="9"/>
+        <v>3586.3</v>
+      </c>
+      <c r="G98">
+        <f t="shared" si="10"/>
+        <v>3455.3078125000002</v>
+      </c>
+      <c r="I98" t="str">
+        <f t="shared" si="11"/>
+        <v>3455,</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>153</v>
+      </c>
+      <c r="B99">
+        <f t="shared" si="6"/>
+        <v>148.19999999999999</v>
+      </c>
+      <c r="C99">
+        <f t="shared" si="7"/>
+        <v>3400</v>
+      </c>
+      <c r="D99">
+        <f t="shared" si="8"/>
+        <v>161</v>
+      </c>
+      <c r="E99">
+        <f t="shared" si="9"/>
+        <v>3586.3</v>
+      </c>
+      <c r="G99">
+        <f t="shared" si="10"/>
+        <v>3469.8625000000002</v>
+      </c>
+      <c r="I99" t="str">
+        <f t="shared" si="11"/>
+        <v>3469,</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>154</v>
+      </c>
+      <c r="B100">
+        <f t="shared" si="6"/>
+        <v>148.19999999999999</v>
+      </c>
+      <c r="C100">
+        <f t="shared" si="7"/>
+        <v>3400</v>
+      </c>
+      <c r="D100">
+        <f t="shared" si="8"/>
+        <v>161</v>
+      </c>
+      <c r="E100">
+        <f t="shared" si="9"/>
+        <v>3586.3</v>
+      </c>
+      <c r="G100">
+        <f t="shared" si="10"/>
+        <v>3484.4171875000002</v>
+      </c>
+      <c r="I100" t="str">
+        <f t="shared" si="11"/>
+        <v>3484,</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>155</v>
+      </c>
+      <c r="B101">
+        <f t="shared" si="6"/>
+        <v>148.19999999999999</v>
+      </c>
+      <c r="C101">
+        <f t="shared" si="7"/>
+        <v>3400</v>
+      </c>
+      <c r="D101">
+        <f t="shared" si="8"/>
+        <v>161</v>
+      </c>
+      <c r="E101">
+        <f t="shared" si="9"/>
+        <v>3586.3</v>
+      </c>
+      <c r="G101">
+        <f t="shared" si="10"/>
+        <v>3498.9718750000002</v>
+      </c>
+      <c r="I101" t="str">
+        <f t="shared" si="11"/>
+        <v>3498,</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>156</v>
+      </c>
+      <c r="B102">
+        <f t="shared" si="6"/>
+        <v>148.19999999999999</v>
+      </c>
+      <c r="C102">
+        <f t="shared" si="7"/>
+        <v>3400</v>
+      </c>
+      <c r="D102">
+        <f t="shared" si="8"/>
+        <v>161</v>
+      </c>
+      <c r="E102">
+        <f t="shared" si="9"/>
+        <v>3586.3</v>
+      </c>
+      <c r="G102">
+        <f t="shared" si="10"/>
+        <v>3513.5265625000002</v>
+      </c>
+      <c r="I102" t="str">
+        <f t="shared" si="11"/>
+        <v>3513,</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>157</v>
+      </c>
+      <c r="B103">
+        <f t="shared" si="6"/>
+        <v>148.19999999999999</v>
+      </c>
+      <c r="C103">
+        <f t="shared" si="7"/>
+        <v>3400</v>
+      </c>
+      <c r="D103">
+        <f t="shared" si="8"/>
+        <v>161</v>
+      </c>
+      <c r="E103">
+        <f t="shared" si="9"/>
+        <v>3586.3</v>
+      </c>
+      <c r="G103">
+        <f t="shared" si="10"/>
+        <v>3528.0812500000002</v>
+      </c>
+      <c r="I103" t="str">
+        <f t="shared" si="11"/>
+        <v>3528,</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>158</v>
+      </c>
+      <c r="B104">
+        <f t="shared" si="6"/>
+        <v>148.19999999999999</v>
+      </c>
+      <c r="C104">
+        <f t="shared" si="7"/>
+        <v>3400</v>
+      </c>
+      <c r="D104">
+        <f t="shared" si="8"/>
+        <v>161</v>
+      </c>
+      <c r="E104">
+        <f t="shared" si="9"/>
+        <v>3586.3</v>
+      </c>
+      <c r="G104">
+        <f t="shared" si="10"/>
+        <v>3542.6359375000002</v>
+      </c>
+      <c r="I104" t="str">
+        <f t="shared" si="11"/>
+        <v>3542,</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>159</v>
+      </c>
+      <c r="B105">
+        <f t="shared" si="6"/>
+        <v>148.19999999999999</v>
+      </c>
+      <c r="C105">
+        <f t="shared" si="7"/>
+        <v>3400</v>
+      </c>
+      <c r="D105">
+        <f t="shared" si="8"/>
+        <v>161</v>
+      </c>
+      <c r="E105">
+        <f t="shared" si="9"/>
+        <v>3586.3</v>
+      </c>
+      <c r="G105">
+        <f t="shared" si="10"/>
+        <v>3557.1906250000002</v>
+      </c>
+      <c r="I105" t="str">
+        <f t="shared" si="11"/>
+        <v>3557,</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>160</v>
+      </c>
+      <c r="B106">
+        <f t="shared" si="6"/>
+        <v>148.19999999999999</v>
+      </c>
+      <c r="C106">
+        <f t="shared" si="7"/>
+        <v>3400</v>
+      </c>
+      <c r="D106">
+        <f t="shared" si="8"/>
+        <v>161</v>
+      </c>
+      <c r="E106">
+        <f t="shared" si="9"/>
+        <v>3586.3</v>
+      </c>
+      <c r="G106">
+        <f t="shared" si="10"/>
+        <v>3571.7453125000002</v>
+      </c>
+      <c r="I106" t="str">
+        <f t="shared" si="11"/>
+        <v>3571,</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I107" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
@@ -543,7 +5426,7 @@
         <v>71</v>
       </c>
       <c r="B16">
-        <f t="shared" ref="B16:B61" si="0">INDEX($A$2:$A$9,MATCH(A16,$A$2:$A$9,1))</f>
+        <f t="shared" ref="B16:B60" si="0">INDEX($A$2:$A$9,MATCH(A16,$A$2:$A$9,1))</f>
         <v>69</v>
       </c>
       <c r="C16">

</xml_diff>